<commit_message>
addec new data source
</commit_message>
<xml_diff>
--- a/data/df_with_many_tags_27_11.xlsx
+++ b/data/df_with_many_tags_27_11.xlsx
@@ -468,12 +468,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Acoustic Control System, Autonomous Underwater Vehicle, acoustic telemetry link, 3D sonar technology, BOP operation, underwater surveillance</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Surveilance &amp; monitoring</t>
+          <t>Surveillance &amp; monitoring</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -495,9 +495,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>{
-  "tags": "GPS receiver, marine echo sounder, GNSS infrastructure, sensor fusion compatible, vessel tracking, maritime navigation"
-}</t>
+          <t>GPS receiver, IALA beacon receiver, GNSS infrastructure, spoofing mitigation, vessel tracking, maritime navigation</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -524,12 +522,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>AIS transponder, acoustic telemetry link, marine survey, remote sensing</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Surveilance &amp; monitoring</t>
+          <t>Surveillance &amp; monitoring</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -551,12 +549,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Acoustic Control System, AIS transponder, remote sensing, marine survey</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Surveilance &amp; monitoring</t>
+          <t>Surveillance &amp; monitoring</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -578,9 +576,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Radio, transceiver, reconfigurable SDR, VDES technology, maritime communication, navigation systems"
-}</t>
+          <t>radio, transceiver, reconfigurable SDR, VDES technology, maritime communication, navigation systems</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -607,9 +603,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Positioning system, Navigation system, acoustic telemetry, Hydroacoustic Positioning, dynamic positioning reference, subsea survey"
-}</t>
+          <t>Positioning system, Navigation system, acoustic telemetry, Hydroacoustic Positioning, dynamic positioning reference, subsea survey</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -636,9 +630,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Positioning system, Navigation system, acoustic telemetry, Hydroacoustic Positioning, dynamic positioning reference, subsea survey"
-}</t>
+          <t>Positioning system, Navigation system, acoustic telemetry, Hydroacoustic Positioning, ROV integration, subsea survey</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -665,12 +657,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Acoustic Control System, Leak Detection System, acoustic telemetry link, autonomous navigation, BOP operation, underwater surveillance</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Surveilance &amp; monitoring</t>
+          <t>Surveillance &amp; monitoring</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -692,11 +684,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>{
-  "Data Management": "Quality Assurance, Industrial IoT",
-  "Technology": "cloud-based, AI classification",
-  "Application": "environmental monitoring, ocean exploration"
-}</t>
+          <t>Data Management, Cloud Storage, cloud-based, AI classification, environmental monitoring, ocean exploration</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -723,9 +711,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echo sounder system, sonar technology, acoustic Doppler, sensor fusion algorithms, scientific research, environmental monitoring"
-}</t>
+          <t>echo sounder system, sonar technology, wideband technology, sensor fusion algorithms, environmental monitoring, fish stock assessment</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -752,12 +738,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Acoustic Control System, AIS transponder, remote sensing, marine survey</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Surveilance &amp; monitoring</t>
+          <t>Surveillance &amp; monitoring</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -779,12 +765,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Acoustic Control System, AIS transponder, underwater surveillance, remote sensing</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Surveilance &amp; monitoring</t>
+          <t>Surveillance &amp; monitoring</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -806,16 +792,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>{"tags": "AUV, advanced navigation system, HISAS, environmental monitoring, subsea mapping, marine survey"}, nan, {
-  "tags": "Autonomous Underwater Vehicle, customizable payload, long endurance, maritime research support, autonomous maritime vehicle"
-}, {"tags": "Sub-bottom profiler, Multibeam sonar, multibeam echosounder, side-scan sonar, seafloor mapping, subsea survey"}, {
-  "tags": "Autonomous Underwater Vehicle, Sub-bottom profiler, advanced navigation system, low frequency transducers, seafloor mapping, geophysical survey"
-}</t>
+          <t>AUV, advanced navigation system, HISAS, environmental monitoring, subsea mapping, maritime surveillance, Autonomous Underwater Vehicle, Acoustic Control System, acoustic telemetry link, autonomous navigation, underwater surveillance, marine survey, Autonomous Underwater Vehicle, Sub-bottom profiler, advanced navigation system, low frequency transducers, seafloor mapping, geophysical survey, Multibeam sonar, Side Scan Sonar, multibeam echosounder, high-resolution sonar, seafloor mapping, subsea survey, Autonomous Underwater Vehicle, customizable payload, maritime research support, autonomous maritime vehicle, long endurance</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Seafloor mapping, Surveilance &amp; monitoring, Naval, Geophysical survey, Autonomous and uncrewed solutions</t>
+          <t>Seafloor mapping, Surveillance &amp; monitoring, Naval, Geophysical survey, Autonomous and uncrewed solutions</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -837,18 +819,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Sub-bottom profiler, Multibeam sonar, multibeam echosounder, sub-bottom profiling, seafloor mapping, subsea survey"
-}, nan, {"tags": "Autonomous Underwater Vehicle, Sub-bottom profiler, advanced navigation system, next generation obstacle avoidance sonar, geophysical survey, seafloor mapping"}, {
-  "tags": "AUV, underwater, 3D sonar technology, advanced navigation system, subsea mapping, marine survey"
-}, {
-  "tags": "Autonomous Underwater Vehicle, Diver Detection Sonar, remote vessel operation, customizable payload, long endurance, maritime research support"
-}</t>
+          <t>AUV, underwater, 3D sonar technology, advanced navigation system, subsea mapping, marine survey, Autonomous Underwater Vehicle, Sub-bottom profiler, advanced navigation system, low frequency transducers, geophysical survey, sediment layer mapping, Autonomous Underwater Vehicle, customizable payload, remote vessel operation, long endurance, autonomous maritime vehicle, maritime research support, Autonomous Underwater Vehicle, Acoustic Control System, 3D sonar technology, autonomous navigation, underwater surveillance, marine survey, Sub-bottom profiler, Multibeam sonar, multibeam echosounder, sub-bottom profiling, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Seafloor mapping, Surveilance &amp; monitoring, Naval, Geophysical survey, Autonomous and uncrewed solutions</t>
+          <t>Seafloor mapping, Surveillance &amp; monitoring, Naval, Geophysical survey, Autonomous and uncrewed solutions</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -870,18 +846,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>{
-  "tags": "AUV, underwater, HISAS, advanced navigation system, subsea mapping, maritime surveillance"
-}, nan, {"tags": "Multibeam sonar, Side Scan Sonar, multibeam echosounder, high-resolution sonar, seafloor mapping, subsea survey"}, {"tags": "Autonomous Underwater Vehicle, USV hydroacoustic applications, long endurance, maritime research support"}, {
-  "product type": ["Autonomous Underwater Vehicle", "Sub-bottom profiler"],
-  "technology": ["advanced navigation system", "sub-bottom sonar"],
-  "application": ["geophysical survey", "seafloor mapping"]
-}</t>
+          <t>Autonomous Underwater Vehicle, advanced navigation system, seafloor mapping, geophysical survey, deep-sea exploration, sub-bottom sonar, Autonomous Underwater Vehicle, 3D sonar technology, acoustic telemetry link, underwater surveillance, marine survey, AUV, underwater, HISAS, advanced navigation system, subsea mapping, maritime surveillance, Autonomous Underwater Vehicle, remote vessel operation, long endurance, maritime research support, autonomous maritime vehicle, customizable payload, Multibeam sonar, Side Scan Sonar, multibeam echosounder, high-resolution sonar, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Seafloor mapping, Surveilance &amp; monitoring, Naval, Geophysical survey, Autonomous and uncrewed solutions</t>
+          <t>Seafloor mapping, Surveillance &amp; monitoring, Naval, Geophysical survey, Autonomous and uncrewed solutions</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -903,12 +873,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>{"tags": "AUV, HISAS, subsea mapping, environmental monitoring, marine survey, maritime surveillance"}, {"tags": "Multibeam sonar, Sub-bottom profiler, multibeam echosounder, sub-bottom profiling, seafloor mapping, subsea survey"}, {"tags": "Autonomous Underwater Vehicle, USV hydroacoustic applications, long endurance, maritime research support, autonomous maritime vehicle"}, nan, {"tags": "Autonomous Underwater Vehicle, Sub-bottom profiler, advanced navigation system, sub-bottom sonar, seafloor mapping, geophysical survey"}</t>
+          <t>Autonomous Underwater Vehicle, Sub-bottom profiler, sub-bottom sonar, advanced navigation system, seafloor mapping, geophysical survey, Autonomous Underwater Vehicle, remote vessel operation, long endurance, maritime research support, autonomous maritime vehicle, AUV, underwater, HISAS, advanced navigation system, environmental monitoring, subsea mapping, Autonomous Underwater Vehicle, Acoustic Control System, 3D sonar technology, autonomous navigation, underwater surveillance, marine survey, Sub-bottom profiler, Multibeam sonar, multibeam echosounder, sub-bottom profiling, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Seafloor mapping, Surveilance &amp; monitoring, Naval, Geophysical survey, Autonomous and uncrewed solutions</t>
+          <t>Seafloor mapping, Surveillance &amp; monitoring, Naval, Geophysical survey, Autonomous and uncrewed solutions</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -930,11 +900,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Navigation system, Positioning system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, ROV integration"
-}, {
-  "tags": "Cloud Storage, Industrial IoT, cloud-based, AI classification, environmental monitoring, data visualization"
-}</t>
+          <t>Positioning system, Navigation system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, subsea survey, Cloud Storage, Data Management, cloud-based, AI classification, data visualization, environmental monitoring</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -961,9 +927,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Data Management, Cloud Storage, cloud-based, Cyber Security, data visualization, situational awareness"
-}</t>
+          <t>Data Management, Cloud Storage, cloud-based, Cyber Security, data visualization, situational awareness</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -990,9 +954,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>{
-  "tags": "GPS receiver, IALA beacon receiver, GNSS infrastructure, spoofing mitigation, GPS, maritime navigation"
-}</t>
+          <t>GPS receiver, IALA beacon receiver, GNSS infrastructure, sensor fusion compatible, GPS, maritime navigation</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1019,9 +981,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Data Management, Cloud Storage, cloud-based, AI classification, environmental monitoring, situational awareness"
-}</t>
+          <t>Data Management, Cloud Storage, cloud-based, AI classification, environmental monitoring, data visualization</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1048,12 +1008,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>nan, {"tags": "Diver Detection Sonar, USV hydroacoustic applications, maritime research support, autonomous maritime vehicle"}</t>
+          <t>Diver Detection Sonar, USV hydroacoustic applications, long endurance, maritime research support, Diver Detection Sonar, 3D sonar technology, underwater surveillance</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Surveilance &amp; monitoring, Naval</t>
+          <t>Surveillance &amp; monitoring, Naval</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1075,12 +1035,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Acoustic Control System, Diver Detection Sonar, 3D sonar technology, acoustic telemetry link, underwater surveillance, marine survey</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Surveilance &amp; monitoring</t>
+          <t>Surveillance &amp; monitoring</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1102,9 +1062,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Multibeam sonar, Sub-bottom profiler, multibeam echosounder, sub-bottom profiling, seafloor mapping, subsea survey"
-}</t>
+          <t>Multibeam sonar, Sub-bottom profiler, multibeam echosounder, sub-bottom profiling, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1131,12 +1089,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Diver Detection Sonar, Acoustic Control System, 3D sonar technology, acoustic telemetry link, underwater surveillance, marine survey</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Surveilance &amp; monitoring</t>
+          <t>Surveillance &amp; monitoring</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1158,9 +1116,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Side Scan Sonar, high-resolution sonar, seafloor mapping, subsea survey"
-}</t>
+          <t>Side Scan Sonar, Single beam echo sounder, side-scan sonar, high-resolution sonar, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1187,11 +1143,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Sub-bottom profiler, low frequency transducers, geophysical survey, sediment layer mapping"
-}, {
-  "tags": "Sub-bottom profiler, Single beam echo sounder, sub-bottom profiling, seafloor mapping, subsea survey"
-}</t>
+          <t>Sub-bottom profiler, Multibeam echosounder software, low frequency transducers, sub-bottom sonar, geophysical survey, sediment layer mapping, Sub-bottom profiler, Single beam echo sounder, sub-bottom profiling, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1218,9 +1170,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Single beam echo sounder, Side Scan Sonar, high-resolution sonar, sub-bottom profiling, seafloor mapping, subsea survey"
-}</t>
+          <t>Single beam echo sounder, Side Scan Sonar, multibeam echosounder, side-scan sonar, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1247,7 +1197,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>{"tags":["Single beam echo sounder","Multibeam sonar","high-resolution sonar","multibeam echosounder","seafloor mapping","subsea survey"]}</t>
+          <t>Single beam echo sounder, Multibeam sonar, high-resolution sonar, multibeam echosounder, seafloor mapping, oceanography</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1274,9 +1224,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>{
-  "tags": "autonomous transceiver, oceanographic instrument, wideband technology, scientific research, environmental monitoring, fish stock assessment"
-}</t>
+          <t>echo sounder system, oceanographic instrument, wideband technology, acoustic Doppler, scientific research, environmental monitoring</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1303,13 +1251,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>{
-  "echo sounder system": "scientific research, environmental monitoring",
-  "wideband technology": "GPS integrated system",
-  "fish stock assessment": "marine navigation"
-}, {
-  "tags": "portable transducer, transceiver marine research, broadband sweeps, frequency adjustment, fish finding, underwater survey"
-}</t>
+          <t>echo sounder system, oceanographic instrument, wideband technology, GPS integrated system, scientific research, environmental monitoring, portable transducer, transceiver marine research, broadband sweeps, frequency adjustment, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1336,11 +1278,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, split-beam transducer, dual frequency, fish finding, underwater survey"
-}, {
-  "tags": "echo sounder system, oceanographic instrument, wideband technology, split-beam transducer, scientific research, environmental monitoring"
-}</t>
+          <t>echosounder transducer, transceiver marine research, split-beam transducer, dual frequency, fish finding, underwater survey, echo sounder system, oceanographic instrument, wideband technology, GPS integrated system, scientific research, environmental monitoring</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1367,13 +1305,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echo sounder system, oceanographic instrument, wideband technology, acoustic Doppler, scientific research, fish stock assessment"
-}, {
-  "product type": "software documentation, transceiver marine research",
-  "technology": "broadband sweeps, frequency adjustment",
-  "application": "fish finding, fish stock assessment"
-}</t>
+          <t>echo sounder system, oceanographic instrument, wideband technology, acoustic Doppler, scientific research, fish stock assessment, software documentation, transceiver marine research, broadband sweeps, frequency adjustment, fish finding, fish stock assessment</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1400,9 +1332,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Multibeam sonar, multibeam echosounder, seafloor mapping, oceanography, deep sea exploration"
-}</t>
+          <t>Multibeam sonar, high-resolution sonar, seafloor mapping, deep sea exploration</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1429,9 +1359,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Multibeam sonar, high-resolution sonar, seafloor mapping, subsea survey, deep sea exploration"
-}</t>
+          <t>Multibeam sonar, high-resolution sonar, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1458,7 +1386,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>{"tags": "Multibeam sonar, multibeam echosounder, seafloor mapping, subsea survey, oceanography"}</t>
+          <t>Multibeam sonar, high-resolution sonar, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1485,9 +1413,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Multibeam sonar, multibeam echosounder, seafloor mapping, subsea survey"
-}</t>
+          <t>Multibeam sonar, high-resolution sonar, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1514,7 +1440,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>{"tags": "Multibeam sonar, multibeam echosounder, seafloor mapping, subsea survey, deep sea exploration, high-resolution sonar"}</t>
+          <t>Multibeam sonar, high-resolution sonar, seafloor mapping, subsea survey, deep sea exploration, oceanography</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1541,9 +1467,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Multibeam sonar, multibeam echosounder, seafloor mapping, subsea survey, high-resolution sonar, oceanography"
-}</t>
+          <t>Multibeam sonar, high-resolution sonar, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1570,9 +1494,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Multibeam sonar, multibeam echosounder, seafloor mapping, subsea survey"
-}</t>
+          <t>Multibeam sonar, multibeam echosounder, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1599,7 +1521,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>{"tags": "Multibeam sonar, multibeam echosounder, seafloor mapping, subsea survey, deep sea exploration, oceanography"}</t>
+          <t>Multibeam sonar, high-resolution sonar, seafloor mapping, subsea survey, deep sea exploration, oceanography</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1626,9 +1548,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Multibeam sonar, multibeam echosounder, seafloor mapping, subsea survey, deep sea exploration"
-}</t>
+          <t>Multibeam sonar, High-resolution sonar, Seafloor mapping, Subsea survey, Deep sea exploration, Oceanography</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1655,11 +1575,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>{
-  "product type": ["Multibeam sonar", "Single beam echo sounder"],
-  "technology": ["multibeam echosounder"],
-  "application": ["seafloor mapping", "subsea survey"]
-}</t>
+          <t>Multibeam sonar, multibeam echosounder, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1686,7 +1602,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>{"tags": "Multibeam sonar, multibeam echosounder, seafloor mapping, subsea survey, deep sea exploration, oceanography"}</t>
+          <t>Multibeam sonar, high-resolution sonar, seafloor mapping, subsea survey, deep sea exploration, oceanography</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1713,9 +1629,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Single beam echo sounder, Sub-bottom profiler, multibeam echosounder, high-resolution sonar, seafloor mapping, subsea survey"
-}</t>
+          <t>Single beam echo sounder, Sub-bottom profiler, multibeam echosounder, high-resolution sonar, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1742,9 +1656,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>{
-  "tags": "oceanographic instrument, acoustic Doppler, environmental monitoring, marine navigation"
-}</t>
+          <t>oceanographic instrument, sonar technology, wideband technology, GPS integrated system, environmental monitoring, fish stock assessment</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1771,9 +1683,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, split-beam transducer, dual frequency, fish finding, underwater survey"
-}</t>
+          <t>echosounder transducer, transceiver marine research, split-beam transducer, dual frequency, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1800,9 +1710,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>{
-  "tags": "GPS receiver, inertial sensor, GNSS infrastructure, sensor fusion compatible, maritime navigation, vessel tracking"
-}</t>
+          <t>GPS receiver, inertial sensor, GNSS infrastructure, sensor fusion compatible, maritime navigation, vessel tracking</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1829,7 +1737,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>{"product type": "GPS receiver, inertial sensor", "technology": "GNSS infrastructure, spoofing mitigation", "application": "vessel tracking, maritime navigation"}</t>
+          <t>GPS receiver, inertial sensor, GNSS infrastructure, spoofing mitigation, maritime navigation, vessel tracking</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1856,9 +1764,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>{
-  "tags": "GPS receiver, inertial sensor, GNSS infrastructure, sensor fusion compatible, maritime navigation, vessel tracking"
-}</t>
+          <t>GPS receiver, inertial sensor, GNSS infrastructure, sensor fusion compatible, vessel tracking, maritime navigation</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1885,7 +1791,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>{"tags": "GPS receiver, IALA beacon receiver, sensor fusion compatible, GNSS infrastructure, GPS, maritime navigation"}</t>
+          <t>GPS receiver, IALA beacon receiver, GNSS infrastructure, sensor fusion compatible, maritime navigation, vessel tracking</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1912,9 +1818,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Positioning system, Navigation system, Inertial Measurement Unit, Hydroacoustic Positioning, dynamic positioning reference, subsea survey"
-}</t>
+          <t>Positioning system, Navigation system, Inertial Measurement Unit, Hydroacoustic Positioning, dynamic positioning reference, subsea survey</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1941,7 +1845,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>{"tags": "High-resolution sonar, Side Scan Sonar, seafloor mapping, subsea survey"}</t>
+          <t>high-resolution sonar, side-scan sonar, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1968,9 +1872,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Positioning system, Navigation system, Hydroacoustic Positioning, acoustic telemetry, dynamic positioning reference, ROV integration"
-}</t>
+          <t>Positioning system, Navigation system, Hydroacoustic Positioning, Inertial Measurement Unit, dynamic positioning reference, subsea survey</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1997,12 +1899,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Leak Detection System, Acoustic Control System, AIS transponder, acoustic telemetry link, remote sensing, underwater surveillance</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Surveilance &amp; monitoring</t>
+          <t>Surveillance &amp; monitoring</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -2024,9 +1926,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Positioning system,Navigation system,acoustic telemetry,Hydroacoustic Positioning,underwater communication,ROV integration"
-}</t>
+          <t>Positioning system, Navigation system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, ROV integration</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2053,9 +1953,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Positioning system, Navigation system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, subsea survey"
-}</t>
+          <t>Positioning system, Navigation system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, subsea survey</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2082,11 +1980,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>{
-  "product type": "Positioning system, Navigation system",
-  "technology": "acoustic telemetry, Hydroacoustic Positioning",
-  "application": "dynamic positioning reference, ROV integration"
-}</t>
+          <t>Positioning system, Navigation system, acoustic telemetry, Hydroacoustic Positioning, dynamic positioning reference, ROV integration</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2113,7 +2007,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>{"tags": "Portable Acoustic Positioning system, Navigation system, acoustic telemetry, Inertial Measurement Unit, dynamic positioning reference, subsea survey"}</t>
+          <t>Positioning system, Navigation system, Inertial Measurement Unit, acoustic telemetry, dynamic positioning reference, subsea survey</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2140,7 +2034,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>{"tags": "Positioning system, Navigation system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, subsea survey"}</t>
+          <t>Positioning system, Navigation system, acoustic telemetry, Hydroacoustic Positioning, dynamic positioning reference, subsea survey</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2167,9 +2061,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Positioning system, Navigation system, acoustic telemetry, Hydroacoustic Positioning, dynamic positioning reference, ROV integration"
-}</t>
+          <t>Positioning system, Navigation system, acoustic telemetry, Hydroacoustic Positioning, dynamic positioning reference, subsea survey</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2196,7 +2088,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>{"Positioning system,Navigation system,acoustic telemetry,Hydroacoustic Positioning,dynamic positioning reference,underwater communication"  : []}</t>
+          <t>Positioning system, Navigation system, acoustic telemetry, Hydroacoustic Positioning, dynamic positioning reference, underwater communication</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2223,9 +2115,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Positioning system, Navigation system, acoustic telemetry, Hydroacoustic Positioning, dynamic positioning reference, subsea survey"
-}</t>
+          <t>Positioning system, Navigation system, acoustic telemetry, Hydroacoustic Positioning, dynamic positioning reference, subsea survey</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2252,7 +2142,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>{"tags": "Positioning system, Navigation system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, subsea survey"}</t>
+          <t>Positioning system, Navigation system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, subsea survey</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2279,9 +2169,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Positioning system, Navigation system, Inertial Measurement Unit, Hydroacoustic Positioning, ROV integration, subsea survey"
-}</t>
+          <t>Positioning system, Navigation system, Inertial Measurement Unit, Hydroacoustic Positioning, ROV integration, Subsea survey</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2308,9 +2196,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Positioning system, Navigation system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, subsea survey"
-}</t>
+          <t>Positioning system, Navigation system, Hydroacoustic Positioning, underwater communication, subsea survey</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2337,16 +2223,12 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>nan, {
-  "tags": "surface, underwater, advanced navigation system, Sunstone, maritime surveillance, Situational Awareness"
-}, {
-  "tags": "inertial sensor, marine echo sounder, sensor fusion compatible, augmented reality, maritime navigation, Situational Awareness"
-}</t>
+          <t>Autonomous Underwater Vehicle, Leak Detection System, 3D sonar technology, acoustic telemetry link, underwater surveillance, remote sensing, inertial sensor, marine echo sounder, sensor fusion compatible, GNSS infrastructure, maritime navigation, Situational Awareness, underwater, surface, advanced navigation system, HISAS, maritime surveillance, subsea mapping</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Surveilance &amp; monitoring, Surface navigation &amp; positioning, Autonomous and uncrewed solutions</t>
+          <t>Surveillance &amp; monitoring, Surface navigation &amp; positioning, Autonomous and uncrewed solutions</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2368,18 +2250,12 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>nan, {
-  "product type": "surface, USV",
-  "technology": "advanced navigation system, HISAS",
-  "application": "maritime surveillance, environmental monitoring"
-}, {
-  "tags": "inertial sensor, marine echo sounder, sensor fusion compatible, augmented reality, maritime navigation, vessel tracking"
-}</t>
+          <t>Acoustic Control System, Leak Detection System, autonomous navigation, AIS transponder, underwater surveillance, remote sensing, surface, advanced navigation system, maritime surveillance, marine survey, inertial sensor, marine echo sounder, augmented reality, sensor fusion compatible, maritime navigation, vessel tracking</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Surveilance &amp; monitoring, Surface navigation &amp; positioning, Autonomous and uncrewed solutions</t>
+          <t>Surveillance &amp; monitoring, Surface navigation &amp; positioning, Autonomous and uncrewed solutions</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2401,9 +2277,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>{
-  "tags": "inertial sensor, marine echo sounder, sensor fusion compatible, augmented reality, GPS, maritime navigation"
-}</t>
+          <t>inertial sensor, marine echo sounder, sensor fusion compatible, augmented reality, vessel tracking, maritime navigation</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2430,9 +2304,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Multibeam sonar, Single beam echo sounder, multibeam echosounder, high-resolution sonar, seafloor mapping, oceanography"
-}</t>
+          <t>Multibeam sonar, Single beam echo sounder, multibeam echosounder, high-resolution sonar, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2459,11 +2331,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>{
-  "Multibeam sonar": "multibeam echosounder, fishery research applications",
-  "Technology": "beamforming software, real-time data acquisition",
-  "Application": "seafloor mapping, biomass estimation"
-}</t>
+          <t>Multibeam sonar, multibeam echosounder, seafloor mapping, oceanography</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2490,11 +2358,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>{
-  "product type": "inertial sensor, marine echo sounder",
-  "technology": "sensor fusion compatible, spoofing mitigation",
-  "application": "vessel tracking, maritime navigation"
-}</t>
+          <t>inertial sensor, marine echo sounder, sensor fusion compatible, GNSS infrastructure, vessel tracking, maritime navigation</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2521,9 +2385,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>{
-  "tags": "inertial sensor, marine echo sounder, sensor fusion compatible, augmented reality, vessel tracking, maritime navigation"
-}</t>
+          <t>inertial sensor, marine echo sounder, GNSS infrastructure, sensor fusion compatible, vessel tracking, maritime navigation</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2550,9 +2412,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Radio, Modem, VDES technology, reconfigurable SDR, maritime communication, navigation systems"
-}</t>
+          <t>Radio, Transceiver, VDES technology, Reconfigurable SDR, Maritime communication, Navigation systems</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2579,11 +2439,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>{
-  "product type": "Positioning system, Navigation system",
-  "technology": "acoustic telemetry, Hydroacoustic Positioning",
-  "application": "underwater communication, ROV integration"
-}</t>
+          <t>Positioning system, Navigation system, acoustic telemetry, Hydroacoustic Positioning, dynamic positioning reference, ROV integration</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2610,12 +2466,12 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Leak Detection System, Acoustic Control System, 3D sonar technology, acoustic telemetry link, underwater surveillance, remote sensing</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Surveilance &amp; monitoring</t>
+          <t>Surveillance &amp; monitoring</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2637,9 +2493,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Motion Reference Unit, MEMS gyro, motion sensor, marine navigation, motion compensation, attitude determination"
-}</t>
+          <t>Motion Reference Unit, MEMS gyro, inertial measurement, motion compensation, marine navigation, motion sensor</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2666,9 +2520,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Multibeam sonar, high-resolution sonar, seafloor mapping, subsea survey, marine engineering, environmental monitoring"
-}</t>
+          <t>Multibeam sonar, high-resolution sonar, seafloor mapping, subsea survey, environmental monitoring, underwater science</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2695,11 +2547,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>{
-  "Multibeam sonar": "Multibeam sonar",
-  "Technology": "multibeam echosounder, high-resolution sonar",
-  "Application": "seafloor mapping, subsea survey"
-}</t>
+          <t>Multibeam sonar, high-resolution sonar, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2726,9 +2574,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Navigation Simulation, inertial measurement, post-processing analysis, marine navigation"
-}, {"tags": "Navigation system, Positioning system, Inertial Measurement Unit, Hydroacoustic Positioning, underwater communication, subsea survey"}</t>
+          <t>Navigation Simulation, inertial measurement, post-processing analysis, marine navigation, motion compensation, Navigation system, Positioning system, Inertial Measurement Unit, Hydroacoustic Positioning, underwater communication, ROV integration</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2755,9 +2601,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>{
-  "tags": "inertial sensor, GPS receiver, sensor fusion compatible, spoofing mitigation, maritime navigation, vessel tracking"
-}</t>
+          <t>inertial sensor, GPS receiver, sensor fusion compatible, spoofing mitigation, vessel tracking, maritime navigation</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2784,13 +2628,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Navigation system, Positioning system, Hydroacoustic Positioning, acoustic telemetry, underwater communication, subsea survey"
-}, {
-  "Data Management": "Industrial IoT, Cloud Storage",
-  "Technology": "cloud-based, sensor data analysis",
-  "Application": "situational awareness, data visualization"
-}</t>
+          <t>Data Management, Industrial IoT, cloud-based, sensor data analysis, environmental monitoring, situational awareness, Positioning system, Navigation system, Hydroacoustic Positioning, dynamic positioning reference, subsea survey, underwater communication</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2817,9 +2655,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>{
-  "tags": "portable transducer, echosounder transducer, split-beam transducer, frequency adjustment, fish finding, underwater survey"
-}</t>
+          <t>portable transducer, echosounder transducer, dual frequency, broadband sweeps, fish finding, hydroacoustic synchronization</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2846,9 +2682,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>{
-  "tags": "portable transducer, echosounder transducer, dual frequency, broadband sweeps, fish finding, hydroacoustic synchronization"
-}</t>
+          <t>echosounder transducer, portable transducer, split-beam transducer, fish finding, hydroacoustic synchronization, underwater survey</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2875,9 +2709,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, split-beam transducer, frequency adjustment, fish finding, hydroacoustic synchronization"
-}</t>
+          <t>echosounder transducer, transceiver marine research, split-beam transducer, frequency adjustment, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2904,9 +2736,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, frequency adjustment, fish finding, underwater survey"
-}</t>
+          <t>portable transducer, echosounder transducer, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2933,9 +2763,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Multibeam sonar, Side Scan Sonar, multibeam echosounder, high-resolution sonar, seafloor mapping, subsea survey"
-}</t>
+          <t>Multibeam sonar, Side Scan Sonar, multibeam echosounder, high-resolution sonar, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2962,9 +2790,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Multibeam sonar, Side Scan Sonar, multibeam echosounder, side-scan sonar, seafloor mapping, subsea survey"
-}</t>
+          <t>Multibeam sonar, Side Scan Sonar, multibeam echosounder, side-scan sonar, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2991,9 +2817,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Single beam echo sounder, high-resolution sonar, seafloor mapping, subsea survey"
-}</t>
+          <t>Single beam echo sounder, high-resolution sonar, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3020,9 +2844,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Positioning system, Navigation system, acoustic telemetry, Hydroacoustic Positioning, dynamic positioning reference, subsea survey"
-}</t>
+          <t>Positioning system, Navigation system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, subsea survey</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3049,10 +2871,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>{"product type": "Multibeam sonar", "technology": "multibeam echosounder", "application": "seafloor mapping"}, {"Multibeam echosounder software," 
- 	: ", pitch and roll stabilization," 
- 	,"seafloor mapping," 
- 	:"geophysical survey"}</t>
+          <t>Multibeam echosounder software, pitch and roll stabilization, seafloor mapping, geophysical survey, Multibeam sonar, multibeam echosounder, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3079,11 +2898,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>{
-  "product type": "Data Management, Industrial IoT",
-  "technology": "sensor data analysis, cloud-based",
-  "application": "environmental monitoring, data visualization"
-}</t>
+          <t>Data Management, Industrial IoT, sensor data analysis, cloud-based, environmental monitoring, data visualization</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3110,9 +2925,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Industrial IoT, Quality Assurance, cloud-based, sensor data analysis, situational awareness, data visualization"
-}</t>
+          <t>Industrial IoT, Quality Assurance, cloud-based, sensor data analysis, situational awareness, data visualization</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3139,9 +2952,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Multibeam sonar, Side Scan Sonar, multibeam echosounder, side-scan sonar, seafloor mapping, subsea survey"
-}</t>
+          <t>Multibeam sonar, Side Scan Sonar, multibeam echosounder, side-scan sonar, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -3168,9 +2979,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Side Scan Sonar, Single beam echo sounder, side-scan sonar, high-resolution sonar, seafloor mapping, subsea survey"
-}</t>
+          <t>Side Scan Sonar, Single beam echo sounder, side-scan sonar, high-resolution sonar, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3197,9 +3006,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Side Scan Sonar, high-resolution sonar, seafloor mapping, subsea survey"
-}</t>
+          <t>Side Scan Sonar, high-resolution sonar, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -3226,15 +3033,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>{
-  "product type": "echo sounder system, sonar technology",
-  "technology": "split-beam transducer",
-  "application": "scientific research, deep water measurements"
-}, {
-  "tags": "echosounder transducer, split-beam transducer, fish finding, underwater survey"
-}, {
-  "tags": "Single beam echo sounder, Sub-bottom profiler, multibeam echosounder, sub-bottom profiling, seafloor mapping, deep sea exploration"
-}</t>
+          <t>echosounder transducer, transceiver marine research, dual frequency, split-beam transducer, fish finding, underwater survey, Single beam echo sounder, Multibeam sonar, high-resolution sonar, sub-bottom profiling, seafloor mapping, subsea survey, echo sounder system, oceanographic instrument, acoustic Doppler, split-beam transducer, scientific research, environmental monitoring</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3261,9 +3060,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, single-beam transducer, fish finding, underwater survey"
-}</t>
+          <t>echosounder transducer, frequency adjustment, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3290,9 +3087,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, frequency adjustment, fish finding, underwater survey"
-}</t>
+          <t>echosounder transducer, marine research, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -3319,9 +3114,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, broadband sweeps, fish finding, underwater survey"
-}</t>
+          <t>echosounder transducer, transceiver marine research, broadband sweeps, frequency adjustment, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3348,9 +3141,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, dual frequency, fish finding, underwater survey"
-}</t>
+          <t>echosounder transducer, transceiver marine research, frequency adjustment, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -3377,9 +3168,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>{
-  "tags": "portable transducer, echosounder transducer, fish finding, underwater survey"
-}</t>
+          <t>portable transducer, echosounder transducer, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -3406,9 +3195,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transducer marine research, frequency adjustment, narrow beam, fish finding, underwater survey"
-}</t>
+          <t>echosounder transducer, transceiver marine research, split-beam transducer, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -3435,14 +3222,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>{
-  "echosounder transducer": "Simrad 38-9",
-  "transceiver marine research": "Simrad 38-9",
-  "split-beam transducer": "Simrad 38-9",
-  "fish finding": "Simrad 38-9",
-  "hydroacoustic synchronization": "Simrad 38-9",
-  "underwater survey": "Simrad 38-9"
-}</t>
+          <t>echosounder transducer, marine research, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -3469,7 +3249,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>{"echosounder transducer, transceiver marine research, dual frequency, fish finding, underwater survey" : "tags"}</t>
+          <t>echosounder transducer, transceiver marine research, dual frequency, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -3496,9 +3276,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, dual frequency, fish finding, underwater survey"
-}</t>
+          <t>echosounder transducer, transceiver marine research, dual frequency, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3525,9 +3303,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, dual frequency, fish finding, bottom discrimination, through hull mounting, discontinued product"
-}</t>
+          <t>echosounder transducer, dual frequency, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3554,7 +3330,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>{"tags": "echosounder transducer, transceiver marine research, fish finding, underwater survey"}</t>
+          <t>echosounder transducer, transceiver marine research, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -3581,9 +3357,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>{
-  "tags": "portable transducer, echosounder transducer, fish finding, underwater survey"
-}</t>
+          <t>portable transducer, echosounder transducer, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -3610,9 +3384,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, fish finding, single-beam transducer, hydroacoustic synchronization"
-}</t>
+          <t>echosounder transducer, transceiver marine research, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3639,7 +3411,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>{"tags": "echosounder transducer, transceiver marine research, dual frequency, fish finding, underwater survey"}</t>
+          <t>echosounder transducer, transceiver marine research, dual frequency, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -3666,10 +3438,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>{
-  "echosounder transducer": "dual frequency",
-  "fish finding": "hydroacoustic synchronization"
-}</t>
+          <t>echosounder transducer, transceiver marine research, dual frequency, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -3696,11 +3465,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Radio, Modem, VDES technology, reconfigurable SDR, maritime communication, navigation systems"
-}, {
-  "tags": "echosounder transducer, transceiver marine research, broadband sweeps, frequency adjustment, fish finding, underwater survey"
-}</t>
+          <t>Radio, Transceiver, VDES technology, Reconfigurable SDR, Maritime communication, Navigation systems, transceiver, marine research, broadband sweeps, frequency adjustment, fish finding, hydroacoustic synchronization</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -3727,13 +3492,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, broadband sweeps, fish finding, underwater survey"
-}, {
-  "tags": "echo sounder system, oceanographic instrument, wideband technology, split-beam transducer, scientific research, fish stock assessment"
-}, {
-  "tags": "echosounder transducer, transceiver marine research, broadband sweeps, frequency adjustment, fish finding, underwater survey"
-}</t>
+          <t>echo sounder system, oceanographic instrument, wideband technology, scientific research, environmental monitoring, fish stock assessment, echosounder transducer, transceiver marine research, broadband sweeps, frequency adjustment, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -3760,11 +3519,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>{"tags": "Multibeam echosounder software, Underwater Altimeters, advanced navigation system, pitch and roll stabilization, geophysical survey, seafloor mapping"}, {
-  "tags": "echosounder transducer, transceiver marine research, split-beam transducer, fish finding, underwater survey"
-}, {
-  "tags": "Single beam echo sounder, high-resolution sonar, seafloor mapping, subsea survey"
-}</t>
+          <t>Single beam echo sounder, high-resolution sonar, seafloor mapping, subsea survey, echosounder transducer, transceiver marine research, split-beam transducer, fish finding, underwater survey, hydroacoustic synchronization, Multibeam echosounder software, Underwater Altimeters, low frequency transducers, pitch and roll stabilization, seafloor mapping, geophysical survey</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -3791,9 +3546,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, dual frequency, broadband sweeps, fish finding, hydroacoustic synchronization"
-}</t>
+          <t>echosounder transducer, transceiver marine research, dual frequency, fish finding, hydroacoustic synchronization, underwater survey</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -3820,9 +3573,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, broadband sweeps, frequency adjustment, fish finding, hydroacoustic synchronization"
-}</t>
+          <t>echosounder transducer, transceiver marine research, broadband sweeps, frequency adjustment, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -3849,9 +3600,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echo sounder system, oceanographic instrument, acoustic Doppler, split-beam transducer, scientific research, environmental monitoring"
-}</t>
+          <t>echo sounder system, oceanographic instrument, acoustic Doppler, split-beam transducer, scientific research, environmental monitoring</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -3878,9 +3627,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, split-beam transducer, dual frequency, fish finding, fish stock assessment"
-}</t>
+          <t>echosounder transducer, transceiver marine research, split-beam transducer, dual frequency, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -3907,11 +3654,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>{
-  "product type": "echosounder transducer, transceiver marine research",
-  "technology": "split-beam transducer, dual frequency",
-  "application": "fish finding, fish stock assessment"
-}</t>
+          <t>software documentation, transceiver marine research, split-beam transducer, frequency adjustment, fish finding, hydroacoustic synchronization</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -3938,9 +3681,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, split-beam transducer, fish finding, underwater survey"
-}, {"tags": "oceanographic instrument, autonomous transceiver, wideband technology, split-beam transducer, scientific research, environmental monitoring"}</t>
+          <t>echosounder transducer, transceiver marine research, split-beam transducer, broadband sweeps, fish finding, underwater survey, echo sounder system, oceanographic instrument, wideband technology, split-beam transducer, scientific research, environmental monitoring</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -3967,11 +3708,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echo sounder system, oceanographic instrument, wideband technology, split-beam transducer, scientific research, fish stock assessment"
-}, {
-  "tags": "echosounder transducer, transceiver marine research, split-beam transducer, fish finding, fish stock assessment, underwater survey"
-}</t>
+          <t>echosounder transducer, marine research, split-beam transducer, fish finding, fish stock assessment, underwater survey, oceanographic instrument, echo sounder system, wideband technology, split-beam transducer, scientific research, environmental monitoring</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -3998,9 +3735,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, split-beam transducer, frequency adjustment, fish finding, underwater survey"
-}, {"tags": "echo sounder system, oceanographic instrument, split-beam transducer, wideband technology, scientific research, environmental monitoring"}</t>
+          <t>echo sounder system, oceanographic instrument, split-beam transducer, scientific research, environmental monitoring, fish stock assessment, echosounder transducer, split-beam transducer, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -4027,11 +3762,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, split-beam transducer, fish finding, deep water installations"
-}, {
-  "tags": "echo sounder system, oceanographic instrument, split-beam transducer, scientific research, fish stock assessment"
-}</t>
+          <t>echosounder transducer, transceiver marine research, split-beam transducer, fish finding, underwater survey, echo sounder system, sonar technology, split-beam transducer, scientific research, environmental monitoring, fish stock assessment</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -4058,7 +3789,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>{"tags": "echo sounder system, sonar technology, split-beam transducer, scientific research, environmental monitoring, fish stock assessment"}, {"product_type": "echosounder transducer, portable transducer", "technology": "split-beam transducer", "application": "fish finding, underwater survey"}</t>
+          <t>portable transducer, echosounder transducer, split-beam transducer, fish finding, hydroacoustic synchronization, fish stock assessment, echo sounder system, split-beam transducer, scientific research, fish stock assessment</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -4085,9 +3816,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echo sounder system, oceanographic instrument, split-beam transducer, scientific research, environmental monitoring, deep water measurements"
-}, {"tags": "echosounder transducer, transceiver marine research, split-beam transducer, frequency adjustment, fish finding, underwater survey"}</t>
+          <t>echo sounder system, oceanographic instrument, split-beam transducer, scientific research, environmental monitoring, fish stock assessment, echosounder transducer, frequency adjustment, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -4114,11 +3843,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, broadband sweeps, fish finding, fish stock assessment"
-}, {
-  "tags": "echo sounder system, oceanographic instrument, wideband technology, split-beam transducer, scientific research, fish stock assessment"
-}</t>
+          <t>echo sounder system, oceanographic instrument, wideband technology, split-beam transducer, scientific research, fish stock assessment, echosounder transducer, transceiver marine research, split-beam transducer, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -4145,11 +3870,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, split-beam transducer, frequency adjustment, fish finding, underwater survey"
-}, {
-  "tags": "oceanographic instrument, split-beam transducer, scientific research, fish stock assessment"
-}</t>
+          <t>echosounder transducer, marine research, split-beam transducer, broadband sweeps, fish finding, underwater survey, echo sounder system, oceanographic instrument, split-beam transducer, scientific research, environmental monitoring, fish stock assessment</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -4176,11 +3897,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echo sounder system, oceanographic instrument, split-beam transducer, scientific research, environmental monitoring, fish stock assessment"
-}, {
-  "tags": "echosounder transducer, transceiver marine research, split-beam transducer, frequency adjustment, fish finding, underwater survey"
-}</t>
+          <t>echosounder transducer, transceiver marine research, split-beam transducer, fish finding, underwater survey, hydroacoustic synchronization, echo sounder system, oceanographic instrument, split-beam transducer, scientific research, environmental monitoring, fish stock assessment</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -4207,11 +3924,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echo sounder system, oceanographic instrument, wideband technology, split-beam transducer, scientific research, fish stock assessment"
-}, {
-  "tags": "echosounder transducer, marine research, split-beam transducer, fish finding, underwater survey"
-}</t>
+          <t>echo sounder system, oceanographic instrument, wideband technology, split-beam transducer, scientific research, fish stock assessment, echosounder transducer, transceiver marine research, split-beam transducer, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -4238,9 +3951,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>{"tags": "echosounder transducer, transceiver marine research, split-beam transducer, broadband sweeps, fish finding, underwater survey"}, {
-  "tags": "oceanographic instrument, sonar technology, split-beam transducer, wideband technology, scientific research, fish stock assessment"
-}</t>
+          <t>echo sounder system, oceanographic instrument, split-beam transducer, wideband technology, scientific research, fish stock assessment, echosounder transducer, transceiver marine research, split-beam transducer, broadband sweeps, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -4267,9 +3978,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>{"tags": "echo sounder system, autonomous transceiver, split-beam transducer, scientific research, environmental monitoring"}, {
-  "tags": "echosounder transducer, transceiver marine research, split-beam transducer, fish finding, underwater survey"
-}</t>
+          <t>echosounder transducer, transceiver marine research, split-beam transducer, fish finding, underwater survey, echo sounder system, autonomous transceiver, split-beam transducer, scientific research, environmental monitoring, fish stock assessment</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -4296,11 +4005,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, split-beam transducer, fish finding, hydroacoustic synchronization, underwater survey"
-}, {
-  "tags": "echo sounder system, sonar technology, split-beam transducer, scientific research, environmental monitoring, fish stock assessment"
-}</t>
+          <t>echosounder transducer, transceiver marine research, split-beam transducer, fish finding, hydroacoustic synchronization, fish stock assessment, echo sounder system, sonar technology, acoustic Doppler, split-beam transducer, scientific research, fish stock assessment</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -4327,11 +4032,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echo sounder system, sonar technology, acoustic Doppler, scientific research, fish stock assessment, environmental monitoring"
-}, {
-  "tags": "echosounder transducer, transceiver marine research, split-beam transducer, fish finding, underwater survey"
-}</t>
+          <t>echosounder transducer, marine research, split-beam transducer, fish finding, hydroacoustic synchronization, fish stock assessment, echo sounder system, oceanographic instrument, split-beam transducer, scientific research, environmental monitoring, fish stock assessment</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -4358,11 +4059,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, split-beam transducer, dual frequency, fish finding, underwater survey"
-}, {
-  "tags": "echo sounder system, autonomous transceiver, split-beam transducer, acoustic Doppler, scientific research, fish stock assessment"
-}</t>
+          <t>echosounder transducer, transceiver marine research, split-beam transducer, dual frequency, fish finding, underwater survey, echo sounder system, sonar technology, split-beam transducer, acoustic Doppler, scientific research, fish stock assessment</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -4389,11 +4086,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, split-beam transducer, dual frequency, fish finding, underwater survey"
-}, {
-  "tags": "echo sounder system, oceanographic instrument, split-beam transducer, wideband technology, scientific research, fish stock assessment"
-}</t>
+          <t>echosounder transducer, transceiver marine research, split-beam transducer, dual frequency, fish finding, underwater survey, echo sounder system, oceanographic instrument, split-beam transducer, scientific research, fish stock assessment, environmental monitoring</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -4420,9 +4113,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echo sounder system, sonar technology, split-beam transducer, scientific research, fish stock assessment, environmental monitoring"
-}, {"echosounder transducer, marine research, split-beam transducer, fish finding, hydroacoustic synchronization, fish stock assessment"  : true}</t>
+          <t>echosounder transducer, portable transducer, split-beam transducer, fish finding, fish stock assessment, underwater survey, echo sounder system, sonar technology, split-beam transducer, scientific research, environmental monitoring, fish stock assessment</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -4449,7 +4140,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>{"tags": "echosounder transducer, marine research, split-beam transducer, fish finding, fish stock assessment, underwater survey"}, {"tags": "echo sounder system, sonar technology, split-beam transducer, scientific research, fish stock assessment"}</t>
+          <t>echo sounder system, oceanographic instrument, split-beam transducer, wideband technology, scientific research, fish stock assessment, echosounder transducer, transceiver marine research, split-beam transducer, fish finding, fish stock assessment, underwater survey</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -4476,11 +4167,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, split-beam transducer, fish finding, underwater survey"
-}, {
-  "tags": "echo sounder system, sonar technology, split-beam transducer, scientific research, fish stock assessment"
-}</t>
+          <t>echosounder transducer, transceiver marine research, split-beam transducer, fish finding, underwater survey, echo sounder system, oceanographic instrument, split-beam transducer, scientific research, fish stock assessment</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -4507,9 +4194,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>{"tags": "echosounder transducer, marine research, split-beam transducer, fish finding, fish stock assessment"}, {
-  "tags": "echo sounder system, sonar technology, split-beam transducer, scientific research, fish stock assessment"
-}</t>
+          <t>echosounder transducer, marine research, split-beam transducer, fish finding, fish stock assessment, echo sounder system, split-beam transducer, scientific research, fish stock assessment</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -4536,9 +4221,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, split-beam transducer, dual frequency, fish finding, fish stock assessment"
-}, {"tags": "echo sounder system, sonar technology, split-beam transducer, scientific research, fish stock assessment, marine navigation"}</t>
+          <t>echo sounder system, oceanographic instrument, split-beam transducer, wideband technology, scientific research, fish stock assessment, echosounder transducer, transceiver marine research, split-beam transducer, frequency adjustment, fish finding, fish stock assessment</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -4565,11 +4248,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>{
-  "tags": "sonar technology, oceanographic instrument, split-beam transducer, scientific research, fish stock assessment"
-}, {
-  "tags": "echosounder transducer, marine research, split-beam transducer, fish finding, hydroacoustic synchronization, underwater survey"
-}</t>
+          <t>echo sounder system, sonar technology, split-beam transducer, scientific research, fish stock assessment, environmental monitoring, echosounder transducer, marine research, split-beam transducer, frequency adjustment, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -4596,11 +4275,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>{
-  "tags": "oceanographic instrument, split-beam transducer, scientific research, environmental monitoring"
-}, {
-  "tags": "echosounder transducer, marine research, split-beam transducer, broadband sweeps, fish finding, underwater survey"
-}</t>
+          <t>echosounder transducer, transceiver marine research, split-beam transducer, broadband sweeps, fish finding, underwater survey, echo sounder system, oceanographic instrument, split-beam transducer, wideband technology, scientific research, environmental monitoring</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -4627,11 +4302,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echo sounder system, split-beam transducer, scientific research, fish stock assessment"
-}, {
-  "tags": "echosounder transducer, transceiver marine research, split-beam transducer, frequency adjustment, fish finding, fish stock assessment"
-}</t>
+          <t>echo sounder system, oceanographic instrument, split-beam transducer, wideband technology, scientific research, fish stock assessment, echosounder transducer, transceiver marine research, split-beam transducer, broadband sweeps, fish finding, fish stock assessment</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -4658,9 +4329,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>{"tags": "echosounder transducer, split-beam transducer, fish finding, underwater survey"}, {
-  "tags": "sonar technology, oceanographic instrument, split-beam transducer, scientific research, fish stock assessment"
-}</t>
+          <t>echo sounder system, oceanographic instrument, split-beam transducer, wideband technology, scientific research, fish stock assessment, echosounder transducer, transceiver marine research, split-beam transducer, broadband sweeps, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -4687,11 +4356,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echo sounder system, sonar technology, wideband technology, acoustic Doppler, scientific research, fish stock assessment"
-}, {
-  "tags": "echosounder transducer, transceiver marine research, split-beam transducer, broadband sweeps, fish finding, underwater survey"
-}</t>
+          <t>echosounder transducer, transceiver marine research, split-beam transducer, broadband sweeps, fish finding, underwater survey, echo sounder system, sonar technology, wideband technology, acoustic Doppler, scientific research, environmental monitoring</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -4718,9 +4383,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, split-beam transducer, broadband sweeps, fish finding, fish stock assessment"
-}</t>
+          <t>portable transducer, echosounder transducer, split-beam transducer, dual frequency, fish finding, fish stock assessment</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -4747,9 +4410,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, broadband sweeps, frequency adjustment, fish finding, hydroacoustic synchronization"
-}</t>
+          <t>echosounder transducer, transceiver marine research, broadband sweeps, frequency adjustment, fish finding, hydroacoustic synchronization</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -4776,9 +4437,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, dual frequency, hydroacoustic synchronization, fish finding, underwater survey"
-}</t>
+          <t>echosounder transducer, transceiver marine research, split-beam transducer, broadband sweeps, fish finding, hydroacoustic synchronization</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -4805,9 +4464,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, broadband sweeps, frequency adjustment, fish finding, underwater survey"
-}</t>
+          <t>echosounder transducer, transceiver marine research, broadband sweeps, frequency adjustment, fish finding, fish stock assessment</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -4834,11 +4491,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>{
-  "product type": "echosounder transducer, transceiver marine research",
-  "technology": "broadband sweeps, frequency adjustment",
-  "application": "fish finding, underwater survey"
-}</t>
+          <t>transceiver marine research, echosounder transducer, broadband sweeps, frequency adjustment, fish finding, hydroacoustic synchronization</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -4865,9 +4518,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, split-beam transducer, frequency adjustment, fish finding, hydroacoustic synchronization"
-}</t>
+          <t>echosounder transducer, transceiver marine research, split-beam transducer, frequency adjustment, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -4894,9 +4545,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>{
-  "tags": "software documentation, transceiver marine research, frequency adjustment, fish finding, hydroacoustic synchronization"
-}</t>
+          <t>software documentation, transceiver marine research, frequency adjustment, hydroacoustic synchronization, fish stock assessment, underwater survey</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -4923,7 +4572,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>{"tags": "transceiver marine research, echosounder transducer, frequency adjustment, broadband sweeps, fish finding, underwater survey"}</t>
+          <t>transceiver marine research, echosounder transducer, broadband sweeps, frequency adjustment, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -4950,9 +4599,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>{"tags": "software documentation, transceiver marine research, frequency adjustment, hydroacoustic synchronization, fish finding, underwater survey"}, {
-  "tags": "software documentation, sensor programming cable, fish finding, fish stock assessment"
-}</t>
+          <t>software documentation, transceiver marine research, frequency adjustment, fish finding, hydroacoustic synchronization, fish stock assessment, software documentation, transceiver marine research, broadband sweeps, frequency adjustment, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -4979,9 +4626,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, broadband sweeps, frequency adjustment, fish finding, underwater survey"
-}</t>
+          <t>echosounder transducer, transceiver marine research, broadband sweeps, frequency adjustment, fish finding, hydroacoustic synchronization</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -5008,11 +4653,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>{
-  "product type": "software documentation, echosounder transducer",
-  "technology": "broadband sweeps, frequency adjustment",
-  "application": "fish finding, underwater survey"
-}</t>
+          <t>software documentation, transceiver marine research, broadband sweeps, frequency adjustment, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -5039,9 +4680,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, split-beam transducer, broadband sweeps, fish finding, hydroacoustic synchronization"
-}</t>
+          <t>echosounder transducer, software documentation, split-beam transducer, broadband sweeps, fish finding, hydroacoustic synchronization</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -5068,11 +4707,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>{
-  "product type": "echosounder transducer, transceiver marine research",
-  "technology": "split-beam transducer, frequency adjustment",
-  "application": "fish finding, hydroacoustic synchronization"
-}</t>
+          <t>echosounder transducer, software documentation, split-beam transducer, frequency adjustment, fish finding, hydroacoustic synchronization</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -5099,9 +4734,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, broadband sweeps, frequency adjustment, fish finding, underwater survey"
-}</t>
+          <t>echosounder transducer, transceiver marine research, broadband sweeps, frequency adjustment, fish finding, hydroacoustic synchronization</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -5128,9 +4761,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, software documentation, broadband sweeps, frequency adjustment, fish finding, underwater survey"
-}</t>
+          <t>echosounder transducer, software documentation, split-beam transducer, frequency adjustment, fish finding, hydroacoustic synchronization</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
@@ -5157,9 +4788,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, dual frequency, broadband sweeps, fish finding, underwater survey"
-}</t>
+          <t>echosounder transducer, transceiver marine research, split-beam transducer, dual frequency, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
@@ -5186,9 +4815,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, frequency adjustment, broadband sweeps, fish finding, underwater survey"
-}</t>
+          <t>echosounder transducer, transceiver marine research, frequency adjustment, broadband sweeps, fish finding, fish stock assessment</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -5215,11 +4842,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>{
-  "echosounder transducer": "fish finding",
-  "transceiver marine research": "broadband sweeps",
-  "fish finding": "underwater survey"
-}</t>
+          <t>echosounder transducer, transceiver marine research, broadband sweeps, frequency adjustment, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -5246,9 +4869,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, broadband sweeps, frequency adjustment, fish finding, underwater survey"
-}</t>
+          <t>echosounder transducer, transceiver marine research, broadband sweeps, frequency adjustment, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -5275,9 +4896,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, frequency adjustment, fish finding, underwater survey"
-}</t>
+          <t>echosounder transducer, transceiver marine research, frequency adjustment, broadband sweeps, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -5304,11 +4923,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>{
-  "product type": "echosounder transducer, transceiver marine research",
-  "technology": "frequency adjustment, broadband sweeps",
-  "application": "fish finding, fish stock assessment"
-}</t>
+          <t>echosounder transducer, transceiver marine research, broadband sweeps, frequency adjustment, fish finding, underwater survey</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -5335,11 +4950,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>{
-  "product type": "echosounder transducer, transceiver marine research",
-  "technology": "frequency adjustment, broadband sweeps",
-  "application": "fish finding, underwater survey"
-}</t>
+          <t>echosounder transducer, transceiver marine research, frequency adjustment, broadband sweeps, fish finding, hydroacoustic synchronization</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -5366,7 +4977,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>{"tags": "echosounder transducer, transceiver marine research, frequency adjustment, fish finding, fish stock assessment, underwater survey"}</t>
+          <t>echosounder transducer, transceiver marine research, frequency adjustment, fish finding, fish stock assessment, underwater survey</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -5393,7 +5004,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>{"tags": "echosounder transducer, transceiver marine research, frequency adjustment, hydroacoustic synchronization, fish finding, underwater survey"}</t>
+          <t>echosounder transducer, transceiver marine research, broadband sweeps, frequency adjustment, fish finding, hydroacoustic synchronization</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -5420,7 +5031,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>{"product type": "echosounder transducer, transceiver marine research", "technology": "frequency adjustment, broadband sweeps", "application": "fish finding, hydroacoustic synchronization"}</t>
+          <t>echosounder transducer, transceiver marine research, dual frequency, broadband sweeps, fish finding, hydroacoustic synchronization</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -5447,9 +5058,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Single beam echo sounder, Side Scan Sonar, high-resolution sonar, sub-bottom profiling, seafloor mapping, subsea survey"
-}</t>
+          <t>Single beam echo sounder, high-resolution sonar, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -5476,11 +5085,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>{
-  "Single beam echo sounder": "Single beam echo sounder",
-  "Technology": "high-resolution sonar",
-  "Application": "seafloor mapping, deep sea exploration"
-}</t>
+          <t>Single beam echo sounder, seafloor mapping, deep sea exploration</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -5507,9 +5112,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Single beam echo sounder, high-resolution sonar, seafloor mapping, subsea survey"
-}</t>
+          <t>Single beam echo sounder, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -5536,9 +5139,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Single beam echo sounder, high-resolution sonar, seafloor mapping, subsea survey"
-}</t>
+          <t>single beam echo sounder, high-resolution sonar, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -5565,9 +5166,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Side Scan Sonar, Multibeam sonar, side-scan sonar, high-resolution sonar, seafloor mapping, subsea survey"
-}</t>
+          <t>Side Scan Sonar, Multibeam sonar, side-scan sonar, high-resolution sonar, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
@@ -5594,9 +5193,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>{
-  "tags": "sonar software, subsea, underwater mapping, navigation systems"
-}</t>
+          <t>subsea, surface, sonar software, underwater mapping, navigation systems</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
@@ -5623,11 +5220,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Sub-bottom profiler, sub-bottom sonar, seafloor mapping, geophysical survey"
-}, {
-  "tags": "Sub-bottom profiler, GeoPulse, sub-bottom profiling, seafloor mapping, subsea survey"
-}</t>
+          <t>Sub-bottom profiler, sub-bottom profiling, seafloor mapping, subsea survey, Sub-bottom profiler, sub-bottom sonar, geophysical survey, sediment layer mapping</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -5654,13 +5247,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>{
-  "product type": "Sub-bottom profiler",
-  "technology": "sub-bottom profiling",
-  "application": "seafloor mapping, subsea survey"
-}, {
-  "tags": "Sub-bottom profiler, low frequency transducers, geophysical survey, sediment layer mapping"
-}</t>
+          <t>Sub-bottom profiler, sub-bottom sonar, seafloor mapping, geophysical survey, Sub-bottom profiler, sub-bottom profiling, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -5687,13 +5274,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>{
-  "product type": ["Sub-bottom profiler"],
-  "technology": ["sub-bottom sonar", "pitch and roll stabilization"],
-  "application": ["seafloor mapping", "geophysical survey"]
-}, {
-  "tags": "Sub-bottom profiler, Multibeam sonar, sub-bottom profiling, multibeam echosounder, seafloor mapping, deep sea exploration"
-}</t>
+          <t>Sub-bottom profiler, low frequency transducers, pitch and roll stabilization, seafloor mapping, geophysical survey, sediment layer mapping, Sub-bottom profiler, Multibeam sonar, sub-bottom profiling, multibeam echosounder, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
@@ -5720,9 +5301,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>{"tags": "Sub-bottom profiler, low frequency transducers, geophysical survey, sediment layer mapping, seafloor mapping"}, {
-  "tags": "Sub-bottom profiler, Multibeam sonar, sub-bottom profiling, high-resolution sonar, seafloor mapping, subsea survey"
-}</t>
+          <t>Sub-bottom profiler, sub-bottom sonar, geophysical survey, sediment layer mapping, low frequency transducers, deep-sea exploration, Sub-bottom profiler, multibeam echosounder, seafloor mapping, subsea survey, high-resolution sonar, deep sea exploration</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
@@ -5749,11 +5328,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Sub-bottom profiler, Multibeam echosounder software, sub-bottom sonar, low frequency transducers, geophysical survey, sediment layer mapping"
-}, {
-  "tags": "Sub-bottom profiler, Multibeam sonar, sub-bottom profiling, high-resolution sonar, seafloor mapping, subsea survey"
-}</t>
+          <t>Sub-bottom profiler, multibeam echosounder, seafloor mapping, subsea survey, high-resolution sonar, sub-bottom profiling, Sub-bottom profiler, sub-bottom sonar, geophysical survey, sediment layer mapping</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -5780,11 +5355,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Sub-bottom profiler, low frequency transducers, seafloor mapping, geophysical survey, sediment layer mapping"
-}, {
-  "tags": "Sub-bottom profiler, Multibeam sonar, sub-bottom profiling, high-resolution sonar, seafloor mapping, subsea survey"
-}</t>
+          <t>Sub-bottom profiler, low frequency transducers, seafloor mapping, geophysical survey, sediment layer mapping, Sub-bottom profiler, Multibeam sonar, sub-bottom profiling, high-resolution sonar, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -5811,9 +5382,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Sub-bottom profiler, Sub-bottom profiling, Seafloor mapping, Subsea survey"
-}, {"tags": "Sub-bottom profiler, sub-bottom sonar, seafloor mapping, geophysical survey"}</t>
+          <t>Sub-bottom profiler, sub-bottom profiling, seafloor mapping, subsea survey, Sub-bottom profiler, Low frequency transducers, Seafloor mapping, Geophysical survey, Sediment layer mapping</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -5840,9 +5409,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Single beam echo sounder, high-resolution sonar, seafloor mapping, subsea survey"
-}</t>
+          <t>Single beam echo sounder, high-resolution sonar, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
@@ -5869,11 +5436,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>{
-  "product type": "Side Scan Sonar, Multibeam sonar",
-  "technology": "high-resolution sonar, side-scan sonar",
-  "application": "seafloor mapping, subsea survey"
-}</t>
+          <t>Side Scan Sonar, High-resolution sonar, seafloor mapping, subsea survey</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -5900,7 +5463,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>{"tags": "oceanographic instrument, acoustic Doppler, scientific research, environmental monitoring"}</t>
+          <t>oceanographic instrument, autonomous transceiver, GPS integrated system, wideband technology, scientific research, environmental monitoring</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -5927,9 +5490,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Multibeam sonar, 3D Visualization Tool, multibeam echosounder, seafloor mapping, subsea survey, oceanography"
-}</t>
+          <t>Multibeam sonar, 3D Visualization Tool, multibeam echosounder, seafloor mapping, subsea survey, oceanography</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
@@ -5956,7 +5517,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>{"product type": "Transponder, Positioning system", "technology": "acoustic telemetry, Hydroacoustic Positioning", "application": "underwater communication, subsea survey"}</t>
+          <t>Transponder, Navigation system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, subsea survey</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
@@ -5983,7 +5544,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>{"product_type": "USV, surface", "technology": "advanced navigation system, 3D sonar technology", "application": "marine survey, maritime surveillance"}, {"tags": "oceanographic instrument, autonomous transceiver, GPS integrated system, acoustic Doppler, scientific research, environmental monitoring"}, {"tags": "Multibeam sonar, high-resolution sonar, seafloor mapping, subsea survey"}, {"tags": "Uncrewed Surface Vehicle, USV hydroacoustic applications, long endurance, maritime research support, autonomous maritime vehicle"}</t>
+          <t>Multibeam sonar, Single beam echo sounder, multibeam echosounder, high-resolution sonar, seafloor mapping, subsea survey, echo sounder system, autonomous transceiver, acoustic Doppler, GPS integrated system, scientific research, fish stock assessment, Uncrewed Surface Vehicle, customizable payload, USV hydroacoustic applications, long endurance, maritime research support, autonomous maritime vehicle, USV, surface, advanced navigation system, 3D sonar technology, marine survey, maritime surveillance</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
@@ -6010,18 +5571,12 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>nan, {
-  "tags": "underwater, advanced navigation system, ROV, AUV, subsea mapping, marine survey"
-}, {
-  "tags": "Single beam echo sounder, high-resolution sonar, seafloor mapping, subsea survey, ROV, AUV"
-}, {
-  "tags": "Underwater Altimeters, advanced navigation system, geophysical survey, obstacle avoidance, positioning, below surface monitoring"
-}</t>
+          <t>Single beam echo sounder, high-resolution sonar, seafloor mapping, subsea survey, Underwater Altimeters, Autonomous Underwater Vehicle, advanced navigation system, low frequency transducers, geophysical survey, deep-sea exploration, underwater, advanced navigation system, environmental monitoring, subsea mapping, Autonomous Underwater Vehicle, Acoustic Control System, acoustic telemetry link, autonomous navigation, underwater surveillance, marine survey</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>Geophysical survey, Seafloor mapping, Surveilance &amp; monitoring, Autonomous and uncrewed solutions</t>
+          <t>Geophysical survey, Seafloor mapping, Surveillance &amp; monitoring, Autonomous and uncrewed solutions</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
@@ -6043,9 +5598,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>{
-  "tags": "transceiver, surface, VDES technology, reconfigurable SDR, maritime communication, navigation systems"
-}</t>
+          <t>transceiver, surface, VDES technology, reconfigurable SDR, maritime communication, navigation systems</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
@@ -6072,9 +5625,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>{"marine echo sounder, inertial sensor, GNSS infrastructure, augmented reality, environmental monitoring, maritime navigation" 	:[]}, {
-  "tags": "echo sounder system, oceanographic instrument, wideband technology, split-beam transducer, scientific research, fish stock assessment"
-}</t>
+          <t>echo sounder system, oceanographic instrument, wideband technology, split-beam transducer, scientific research, fish stock assessment, marine echo sounder, inertial sensor, sensor fusion compatible, augmented reality, environmental monitoring, maritime navigation</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
@@ -6101,7 +5652,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>{"product type": "marine echo sounder", "technology": "sensor fusion compatible", "application": "maritime navigation, environmental monitoring"}, {"product type": "echo sounder system, autonomous transceiver", "technology": "wideband technology, split-beam transducer", "application": "scientific research, fish stock assessment"}</t>
+          <t>echo sounder system, oceanographic instrument, wideband technology, split-beam transducer, scientific research, fish stock assessment, marine echo sounder, GNSS infrastructure, maritime navigation, environmental monitoring</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
@@ -6128,11 +5679,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echo sounder system, autonomous transceiver, wideband technology, split-beam transducer, scientific research, environmental monitoring"
-}, {
-  "tags": "marine echo sounder, sensor fusion compatible, environmental monitoring, maritime navigation"
-}</t>
+          <t>marine echo sounder, inertial sensor, sensor fusion compatible, GNSS infrastructure, maritime navigation, environmental monitoring, echo sounder system, autonomous transceiver, wideband technology, split-beam transducer, scientific research, environmental monitoring</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
@@ -6159,11 +5706,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echo sounder system, autonomous transceiver, wideband technology, split-beam transducer, scientific research, environmental monitoring"
-}, {
-  "tags": "marine echo sounder, sensor fusion compatible, environmental monitoring, maritime navigation"
-}</t>
+          <t>marine echo sounder, sensor fusion compatible, environmental monitoring, maritime navigation, echo sounder system, oceanographic instrument, wideband technology, split-beam transducer, scientific research, environmental monitoring</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
@@ -6190,13 +5733,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Modem, acoustic modem, subsea communication, navigation systems"
-}, {
-  "product type": "Modem, Positioning system",
-  "technology": "acoustic telemetry, Hydroacoustic Positioning",
-  "application": "underwater communication, ROV integration"
-}</t>
+          <t>Modem, Positioning system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, ROV integration, Modem, subsea, acoustic modem, navigation systems, maritime communication, subsea communication</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
@@ -6223,13 +5760,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>{
-  "Modem": "subsea, acoustic modem",
-  "Technology": "acoustic modem, sonar software",
-  "Application": "maritime communication, subsea communication"
-}, {
-  "tags": "Modem, Positioning system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, ROV integration"
-}</t>
+          <t>Modem, subsea, acoustic modem, sonar software, maritime communication, subsea communication, Modem, Positioning system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, ROV integration</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
@@ -6256,11 +5787,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>{"tags": "Modem, subsea, acoustic modem, sonar software, subsea communication, navigation systems"}, {
-  "product type": "Modem, Positioning system",
-  "technology": "acoustic telemetry, Hydroacoustic Positioning",
-  "application": "underwater communication, subsea survey"
-}</t>
+          <t>Modem, subsea, acoustic modem, sonar software, subsea communication, navigation systems, Modem, Positioning system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, subsea survey</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
@@ -6287,11 +5814,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>{
-  "Transponder": "Positioning system",
-  "acoustic telemetry": "Hydroacoustic Positioning",
-  "underwater communication": "subsea survey"
-}</t>
+          <t>Transponder, Positioning system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, ROV integration</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
@@ -6318,11 +5841,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>{
-  "product type": "Transponder, Positioning system",
-  "technology": "acoustic telemetry, Hydroacoustic Positioning",
-  "application": "dynamic positioning reference, subsea survey"
-}</t>
+          <t>Transponder, Navigation system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, subsea survey</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
@@ -6349,9 +5868,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Transponder, Positioning system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, subsea survey"
-}</t>
+          <t>Transponder, Positioning system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, subsea survey</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
@@ -6378,7 +5895,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>{"tags": "Transponder, Positioning system, Inertial Measurement Unit, acoustic telemetry, underwater communication, subsea survey"}</t>
+          <t>Transponder, Modem, Inertial Measurement Unit, acoustic telemetry, underwater communication, subsea survey</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
@@ -6405,7 +5922,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>{"Transponder, Positioning system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, subsea survey"  : "tags"}</t>
+          <t>Transponder, Navigation system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, subsea survey</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
@@ -6432,9 +5949,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Transponder, Positioning system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, subsea survey"
-}</t>
+          <t>Transponder, Positioning system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, subsea survey</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
@@ -6461,9 +5976,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Transponder, Positioning system, acoustic telemetry, Hydroacoustic Positioning, dynamic positioning reference, ROV integration"
-}</t>
+          <t>Transponder, Navigation system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, ROV integration</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
@@ -6490,9 +6003,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Transponder, Positioning system, acoustic telemetry, Hydroacoustic Positioning, ROV integration, subsea survey"
-}</t>
+          <t>Transponder, Navigation system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, ROV integration</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
@@ -6519,9 +6030,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Transponder, Positioning system, acoustic telemetry, Hydroacoustic Positioning, ROV integration, subsea survey"
-}</t>
+          <t>Transponder, Positioning system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, ROV integration</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
@@ -6548,9 +6057,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Modem, Positioning system, acoustic telemetry, ROV integration, underwater communication, subsea survey"
-}, {"tags": "Modem, subsea, acoustic modem, live video solution, subsea communication, maritime communication"}</t>
+          <t>Modem, subsea, acoustic modem, live video solution, maritime communication, subsea communication, Modem, Positioning system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, ROV integration</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
@@ -6577,11 +6084,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>{
-  "product type": "Transponder, Positioning system",
-  "technology": "acoustic telemetry, Hydroacoustic Positioning",
-  "application": "ROV integration, subsea survey"
-}</t>
+          <t>Transponder, Positioning system, acoustic telemetry, Hydroacoustic Positioning, ROV integration, subsea survey</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
@@ -6608,9 +6111,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>{
-  "tags": "Positioning system, Navigation system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, ROV integration"
-}</t>
+          <t>Transponder, Positioning system, acoustic telemetry, Hydroacoustic Positioning, underwater communication, ROV integration</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
@@ -6637,11 +6138,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>{
-  "tags": "echosounder transducer, transceiver marine research, split-beam transducer, dual frequency, fish finding, underwater survey"
-}, {
-  "tags": "autonomous transceiver, echo sounder system, wideband technology, split-beam transducer, scientific research, fish stock assessment"
-}</t>
+          <t>echosounder transducer, transceiver marine research, split-beam transducer, dual frequency, fish finding, underwater survey, autonomous transceiver, oceanographic instrument, wideband technology, acoustic Doppler, scientific research, environmental monitoring</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">

</xml_diff>